<commit_message>
This is murali commit
</commit_message>
<xml_diff>
--- a/target/test-classes/Book1.xlsx
+++ b/target/test-classes/Book1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303831\Downloads\Hackthon_project-master\Hackthon_project-master\src\test\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -156,6 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,35 +524,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="27.08984375" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="29.1796875"/>
+    <col min="2" max="2" customWidth="true" width="27.08984375"/>
+    <col min="3" max="3" customWidth="true" width="21.6328125"/>
+    <col min="4" max="4" customWidth="true" width="30.6328125"/>
+    <col min="5" max="5" customWidth="true" width="33.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C2" s="1">
@@ -560,119 +561,119 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>32</v>
       </c>
     </row>

</xml_diff>